<commit_message>
Data driven & BDD examples
</commit_message>
<xml_diff>
--- a/MobileTestApp/src/test/resources/TestData.xlsx
+++ b/MobileTestApp/src/test/resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusufsahin/Projects/floappium/MobileTestApp/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A029230-2FF3-A14D-A1F1-5AD908E87625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA218E2-DF9C-404C-B20B-2BCCEBAF8FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29560" yWindow="1820" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Country</t>
-  </si>
-  <si>
-    <t>ExpectedTotal</t>
   </si>
   <si>
     <t>Jane Doe</t>
@@ -120,16 +117,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,18 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="11" style="4" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -455,50 +444,38 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3">
-        <v>280.97000000000003</v>
+      <c r="C3" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3">
-        <v>280.97000000000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3">
-        <v>280.97000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>